<commit_message>
Project plan and Gantt chart
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart.xlsx
+++ b/Documents/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\Games-Technology-Research-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB5172-4B2E-4A6B-A837-07BDDD6B3C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C384057F-3C48-4AA8-ADC1-7A1667BF7EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Task Name</t>
   </si>
@@ -307,7 +307,13 @@
     <t>Prototype - Basic Ray Marching</t>
   </si>
   <si>
-    <t>Project Plan</t>
+    <t>Ray Marching Implementation (Report)</t>
+  </si>
+  <si>
+    <t>Setup Implementation (Report)</t>
+  </si>
+  <si>
+    <t>Full Project Plan</t>
   </si>
 </sst>
 </file>
@@ -755,9 +761,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Gantt Chart'!$B$5:$B$23</c:f>
+              <c:f>'Basic Gantt Chart'!$B$5:$B$24</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -804,20 +810,26 @@
                   <c:v>Prototype - Setup Project</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Project Plan</c:v>
+                  <c:v>Setup Implementation (Report)</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Prototype - Basic Ray Marching</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Ray Marching Implementation (Report)</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Full Project Plan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Gantt Chart'!$C$5:$C$23</c:f>
+              <c:f>'Basic Gantt Chart'!$C$5:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>44479</c:v>
                 </c:pt>
@@ -864,12 +876,18 @@
                   <c:v>44510</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44510</c:v>
+                  <c:v>44512</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>44512</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>44522</c:v>
+                </c:pt>
                 <c:pt idx="18">
+                  <c:v>44529</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>44510</c:v>
                 </c:pt>
               </c:numCache>
@@ -1142,9 +1160,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Gantt Chart'!$B$5:$B$23</c:f>
+              <c:f>'Basic Gantt Chart'!$B$5:$B$24</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -1191,20 +1209,26 @@
                   <c:v>Prototype - Setup Project</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Project Plan</c:v>
+                  <c:v>Setup Implementation (Report)</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Prototype - Basic Ray Marching</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Ray Marching Implementation (Report)</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Full Project Plan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Gantt Chart'!$E$5:$E$23</c:f>
+              <c:f>'Basic Gantt Chart'!$E$5:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1251,15 +1275,18 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1997,7 +2024,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2416,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,7 +3019,7 @@
         <v>44509</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" ref="E18:E23" si="1">D18-C18</f>
+        <f t="shared" ref="E18:E24" si="1">D18-C18</f>
         <v>1</v>
       </c>
       <c r="F18" s="2"/>
@@ -3051,17 +3078,17 @@
     <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="11">
-        <v>44510</v>
+        <v>44512</v>
       </c>
       <c r="D20" s="11">
-        <v>44512</v>
+        <v>44519</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -3091,11 +3118,11 @@
         <v>44512</v>
       </c>
       <c r="D21" s="11">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" ref="E21" si="2">D21-C21</f>
+        <v>10</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -3118,12 +3145,18 @@
     </row>
     <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="B22" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="11">
+        <v>44522</v>
+      </c>
+      <c r="D22" s="11">
+        <v>44529</v>
+      </c>
       <c r="E22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -3146,16 +3179,18 @@
     </row>
     <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>28</v>
+      </c>
       <c r="C23" s="11">
-        <v>44510</v>
+        <v>44529</v>
       </c>
       <c r="D23" s="11">
-        <v>44510</v>
+        <v>44535</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -3176,12 +3211,19 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="11">
+        <v>44510</v>
+      </c>
+      <c r="D24" s="11">
+        <v>44510</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -3228,10 +3270,10 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3252,7 +3294,7 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3278,28 +3320,28 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -3450,6 +3492,31 @@
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Report implementation up to date, Semester 1 gantt chart finished
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart.xlsx
+++ b/Documents/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\Games-Technology-Research-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C384057F-3C48-4AA8-ADC1-7A1667BF7EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64BD82C-0819-46CF-A13E-4C89D97B2381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Task Name</t>
   </si>
@@ -314,6 +314,30 @@
   </si>
   <si>
     <t>Full Project Plan</t>
+  </si>
+  <si>
+    <t>Lit. Review - Volumetric Objects</t>
+  </si>
+  <si>
+    <t>Lit. Review - Fractal Rendering</t>
+  </si>
+  <si>
+    <t>Lit. Review - Lighting/Shadows</t>
+  </si>
+  <si>
+    <t>Ray Marcher Analysis and Design</t>
+  </si>
+  <si>
+    <t>Lighting Analysis and Design</t>
+  </si>
+  <si>
+    <t>CSG Analysis and Design</t>
+  </si>
+  <si>
+    <t>Lit. Review - CSG/Boolean Operations</t>
+  </si>
+  <si>
+    <t>Begin Lighting/Shadows Implementation</t>
   </si>
 </sst>
 </file>
@@ -761,9 +785,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Gantt Chart'!$B$5:$B$24</c:f>
+              <c:f>'Basic Gantt Chart'!$B$5:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -820,16 +844,40 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Full Project Plan</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Lit. Review - CSG/Boolean Operations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Lit. Review - Volumetric Objects</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Lit. Review - Lighting/Shadows</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Lit. Review - Fractal Rendering</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ray Marcher Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Lighting Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>CSG Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Begin Lighting/Shadows Implementation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Gantt Chart'!$C$5:$C$24</c:f>
+              <c:f>'Basic Gantt Chart'!$C$5:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>44479</c:v>
                 </c:pt>
@@ -864,10 +912,10 @@
                   <c:v>44502</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44505</c:v>
+                  <c:v>44504</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44505</c:v>
+                  <c:v>44506</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>44508</c:v>
@@ -888,7 +936,28 @@
                   <c:v>44529</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44510</c:v>
+                  <c:v>44535</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44538</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44541</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44544</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44547</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44557</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,9 +1229,9 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Gantt Chart'!$B$5:$B$24</c:f>
+              <c:f>'Basic Gantt Chart'!$B$5:$B$31</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -1219,16 +1288,40 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Full Project Plan</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Lit. Review - CSG/Boolean Operations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Lit. Review - Volumetric Objects</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Lit. Review - Lighting/Shadows</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Lit. Review - Fractal Rendering</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ray Marcher Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Lighting Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>CSG Analysis and Design</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Begin Lighting/Shadows Implementation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Gantt Chart'!$E$5:$E$24</c:f>
+              <c:f>'Basic Gantt Chart'!$E$5:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1260,16 +1353,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2</c:v>
@@ -1278,7 +1371,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>7</c:v>
@@ -1287,7 +1380,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2024,7 +2138,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2443,10 +2557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,11 +3028,11 @@
         <v>44502</v>
       </c>
       <c r="D15" s="11">
-        <v>44505</v>
+        <v>44504</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2945,14 +3059,14 @@
         <v>19</v>
       </c>
       <c r="C16" s="11">
-        <v>44505</v>
+        <v>44504</v>
       </c>
       <c r="D16" s="11">
         <v>44506</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -2979,14 +3093,14 @@
         <v>20</v>
       </c>
       <c r="C17" s="11">
-        <v>44505</v>
+        <v>44506</v>
       </c>
       <c r="D17" s="11">
         <v>44508</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3016,11 +3130,11 @@
         <v>44508</v>
       </c>
       <c r="D18" s="11">
-        <v>44509</v>
+        <v>44510</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" ref="E18:E24" si="1">D18-C18</f>
-        <v>1</v>
+        <f t="shared" ref="E18:E31" si="1">D18-C18</f>
+        <v>2</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -3118,11 +3232,11 @@
         <v>44512</v>
       </c>
       <c r="D21" s="11">
-        <v>44522</v>
+        <v>44526</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" ref="E21" si="2">D21-C21</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -3213,16 +3327,18 @@
     </row>
     <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="21"/>
+      <c r="B24" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="C24" s="11">
-        <v>44510</v>
+        <v>44535</v>
       </c>
       <c r="D24" s="11">
-        <v>44510</v>
+        <v>44538</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -3243,12 +3359,21 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="B25" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="11">
+        <v>44538</v>
+      </c>
+      <c r="D25" s="11">
+        <v>44541</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" ref="E25:E30" si="3">D25-C25</f>
+        <v>3</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3268,12 +3393,21 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="B26" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="11">
+        <v>44541</v>
+      </c>
+      <c r="D26" s="11">
+        <v>44544</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3293,12 +3427,21 @@
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="11">
+        <v>44544</v>
+      </c>
+      <c r="D27" s="11">
+        <v>44547</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -3318,12 +3461,21 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="11">
+        <v>44547</v>
+      </c>
+      <c r="D28" s="11">
+        <v>44551</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3343,180 +3495,382 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
+    <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="11">
+        <v>44557</v>
+      </c>
+      <c r="D29" s="11">
+        <v>44561</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="11">
+        <v>44562</v>
+      </c>
+      <c r="D30" s="11">
+        <v>44566</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="11">
+        <v>44566</v>
+      </c>
+      <c r="D31" s="11">
+        <v>44571</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>